<commit_message>
Prepare demo of inputs
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/Introduction.xlsx
+++ b/scenarios/cough/processes/Introduction.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -158,15 +158,76 @@
     <t xml:space="preserve">Ja.</t>
   </si>
   <si>
+    <t xml:space="preserve">GO(date_example)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nein.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUMP(Dropout)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Give me your birthdate. I promise to keep the secret :)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">GO(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">prompt_example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">An example of date picker component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prompt_example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prompt example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Now tell me what is you opinion on medical chatbots!</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO(self)</t>
   </si>
   <si>
-    <t xml:space="preserve">Nein.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUMP(Dropout)</t>
-  </si>
-  <si>
     <t xml:space="preserve">self</t>
   </si>
   <si>
@@ -174,6 +235,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bestätigst du, dass es um ein Medikament für dich selbst/Symptom bei dir selbst geht?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An example of free text input component</t>
   </si>
   <si>
     <t xml:space="preserve">GO(data)</t>
@@ -199,7 +263,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,6 +308,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -324,7 +394,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
@@ -463,17 +533,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="46.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
@@ -561,7 +633,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
@@ -591,7 +663,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -599,109 +671,165 @@
         <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="5"/>
+      <c r="H7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C8" s="7" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
+      <c r="H8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="C9" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="9"/>
       <c r="G9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="H9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
+      <c r="D11" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>24</v>
-      </c>
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="9"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="12"/>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="12"/>
+    </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="13"/>
+      <c r="B17" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>